<commit_message>
generate template tambah tgl lahir di data pengguna
</commit_message>
<xml_diff>
--- a/backend/templates/template_data_kendaraan.xlsx
+++ b/backend/templates/template_data_kendaraan.xlsx
@@ -8,7 +8,8 @@
   </bookViews>
   <sheets>
     <sheet name="Data Kendaraan" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="Instruksi" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="Data Referensi" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="Instruksi" sheetId="3" state="visible" r:id="rId3"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -18,7 +19,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="3">
+  <fonts count="5">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
@@ -27,13 +28,24 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <name val="Arial"/>
       <b val="1"/>
       <color rgb="00FFFFFF"/>
+      <sz val="11"/>
     </font>
     <font>
+      <name val="Arial"/>
+      <b val="1"/>
+      <color rgb="0070AD47"/>
+    </font>
+    <font>
+      <name val="Arial"/>
       <b val="1"/>
       <color rgb="0070AD47"/>
       <sz val="14"/>
+    </font>
+    <font>
+      <name val="Arial"/>
     </font>
   </fonts>
   <fills count="4">
@@ -74,7 +86,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
@@ -82,6 +94,8 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -456,14 +470,14 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col width="22" customWidth="1" min="1" max="1"/>
-    <col width="22" customWidth="1" min="2" max="2"/>
-    <col width="22" customWidth="1" min="3" max="3"/>
-    <col width="22" customWidth="1" min="4" max="4"/>
-    <col width="22" customWidth="1" min="5" max="5"/>
-    <col width="22" customWidth="1" min="6" max="6"/>
-    <col width="22" customWidth="1" min="7" max="7"/>
-    <col width="22" customWidth="1" min="8" max="8"/>
+    <col width="25" customWidth="1" min="1" max="1"/>
+    <col width="25" customWidth="1" min="2" max="2"/>
+    <col width="25" customWidth="1" min="3" max="3"/>
+    <col width="25" customWidth="1" min="4" max="4"/>
+    <col width="25" customWidth="1" min="5" max="5"/>
+    <col width="25" customWidth="1" min="6" max="6"/>
+    <col width="25" customWidth="1" min="7" max="7"/>
+    <col width="25" customWidth="1" min="8" max="8"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -520,14 +534,14 @@
     </row>
   </sheetData>
   <dataValidations count="3">
-    <dataValidation sqref="C2:C1000" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="0" errorTitle="Invalid Tipe" error="Pilih dari daftar tipe kendaraan" type="list">
-      <formula1>"Light Vehicle,Electric Vehicle,Double Cabin,Single Cabin,Bus,Ambulance,Fire Truck,Komando,Truk Sampah"</formula1>
+    <dataValidation sqref="C2:C1000" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="0" errorTitle="Invalid Tipe" error="Pilih dari daftar Tipe Kendaraan yang tersedia" type="list">
+      <formula1>='Data Referensi'!$A$2:$A$13</formula1>
     </dataValidation>
-    <dataValidation sqref="D2:D1000" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="0" errorTitle="Invalid Kategori" error="Pilih salah satu: PT, Travel" type="list">
-      <formula1>"PT,Travel"</formula1>
+    <dataValidation sqref="D2:D1000" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="0" errorTitle="Invalid Kategori" error="Pilih dari daftar Kategori yang tersedia" type="list">
+      <formula1>='Data Referensi'!$B$2:$B$3</formula1>
     </dataValidation>
-    <dataValidation sqref="H2:H1000" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="0" errorTitle="Invalid Shift" error="Pilih salah satu: Shift 1, Shift 2" type="list">
-      <formula1>"Shift 1,Shift 2"</formula1>
+    <dataValidation sqref="H2:H1000" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="0" errorTitle="Invalid Shift" error="Pilih dari daftar Shift yang tersedia" type="list">
+      <formula1>='Data Referensi'!$C$2:$C$4</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -540,7 +554,157 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B24"/>
+  <dimension ref="A1:C13"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <cols>
+    <col width="25" customWidth="1" min="1" max="1"/>
+    <col width="25" customWidth="1" min="2" max="2"/>
+    <col width="25" customWidth="1" min="3" max="3"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="4" t="inlineStr">
+        <is>
+          <t>Tipe Kendaraan</t>
+        </is>
+      </c>
+      <c r="B1" s="4" t="inlineStr">
+        <is>
+          <t>Kategori</t>
+        </is>
+      </c>
+      <c r="C1" s="4" t="inlineStr">
+        <is>
+          <t>Shift Type</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>Light Vehicle</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>PT</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>Shift 1</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Electric Vehicle</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>Travel</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>Shift 2</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Double Cabin</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>Shift 3</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Single Cabin</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Bus</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>Minibus</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>Ambulance</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>Fire Truck</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>Komando</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>Truk Sampah</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>Truk Tangki</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>Pickup</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:B26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -549,11 +713,11 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
     <col width="30" customWidth="1" min="1" max="1"/>
-    <col width="60" customWidth="1" min="2" max="2"/>
+    <col width="65" customWidth="1" min="2" max="2"/>
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="4" t="inlineStr">
+      <c r="A1" s="5" t="inlineStr">
         <is>
           <t>INSTRUKSI UPLOAD DATA KENDARAAN</t>
         </is>
@@ -561,166 +725,182 @@
       <c r="B1" t="inlineStr"/>
     </row>
     <row r="2">
-      <c r="A2" t="inlineStr"/>
-      <c r="B2" t="inlineStr"/>
+      <c r="A2" s="6" t="inlineStr"/>
+      <c r="B2" s="6" t="inlineStr"/>
     </row>
     <row r="3">
-      <c r="A3" t="inlineStr">
+      <c r="A3" s="6" t="inlineStr">
         <is>
           <t>1. Format File:</t>
         </is>
       </c>
-      <c r="B3" t="inlineStr"/>
+      <c r="B3" s="6" t="inlineStr"/>
     </row>
     <row r="4">
-      <c r="A4" t="inlineStr"/>
-      <c r="B4" t="inlineStr">
+      <c r="A4" s="6" t="inlineStr"/>
+      <c r="B4" s="6" t="inlineStr">
         <is>
           <t>- Simpan file sebagai .xlsx (Excel)</t>
         </is>
       </c>
     </row>
     <row r="5">
-      <c r="A5" t="inlineStr"/>
-      <c r="B5" t="inlineStr">
+      <c r="A5" s="6" t="inlineStr"/>
+      <c r="B5" s="6" t="inlineStr">
         <is>
           <t>- Jangan ubah nama kolom header</t>
         </is>
       </c>
     </row>
     <row r="6">
-      <c r="A6" t="inlineStr"/>
-      <c r="B6" t="inlineStr"/>
+      <c r="A6" s="6" t="inlineStr"/>
+      <c r="B6" s="6" t="inlineStr"/>
     </row>
     <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>2. Kolom Wajib (*:</t>
-        </is>
-      </c>
-      <c r="B7" t="inlineStr"/>
+      <c r="A7" s="6" t="inlineStr">
+        <is>
+          <t>2. Kolom Wajib (*):</t>
+        </is>
+      </c>
+      <c r="B7" s="6" t="inlineStr"/>
     </row>
     <row r="8">
-      <c r="A8" t="inlineStr"/>
-      <c r="B8" t="inlineStr">
+      <c r="A8" s="6" t="inlineStr"/>
+      <c r="B8" s="6" t="inlineStr">
         <is>
           <t>- Nomor Polisi: Format standar (contoh: KT 1234 AB)</t>
         </is>
       </c>
     </row>
     <row r="9">
-      <c r="A9" t="inlineStr"/>
-      <c r="B9" t="inlineStr">
+      <c r="A9" s="6" t="inlineStr"/>
+      <c r="B9" s="6" t="inlineStr">
         <is>
           <t>- Tipe Kendaraan: Pilih dari dropdown</t>
         </is>
       </c>
     </row>
     <row r="10">
-      <c r="A10" t="inlineStr"/>
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>- Kategori: PT atau Travel</t>
+      <c r="A10" s="6" t="inlineStr"/>
+      <c r="B10" s="6" t="inlineStr">
+        <is>
+          <t>- Kategori: Pilih dari dropdown (PT/Travel)</t>
         </is>
       </c>
     </row>
     <row r="11">
-      <c r="A11" t="inlineStr"/>
-      <c r="B11" t="inlineStr">
-        <is>
-          <t>- Shift Type: Shift 1 atau Shift 2</t>
+      <c r="A11" s="6" t="inlineStr"/>
+      <c r="B11" s="6" t="inlineStr">
+        <is>
+          <t>- Shift Type: Pilih dari dropdown</t>
         </is>
       </c>
     </row>
     <row r="12">
-      <c r="A12" t="inlineStr"/>
-      <c r="B12" t="inlineStr"/>
+      <c r="A12" s="6" t="inlineStr"/>
+      <c r="B12" s="6" t="inlineStr"/>
     </row>
     <row r="13">
-      <c r="A13" t="inlineStr">
+      <c r="A13" s="6" t="inlineStr">
         <is>
           <t>3. Kolom Opsional:</t>
         </is>
       </c>
-      <c r="B13" t="inlineStr"/>
+      <c r="B13" s="6" t="inlineStr"/>
     </row>
     <row r="14">
-      <c r="A14" t="inlineStr"/>
-      <c r="B14" t="inlineStr">
+      <c r="A14" s="6" t="inlineStr"/>
+      <c r="B14" s="6" t="inlineStr">
         <is>
           <t>- Nomor Lambung: Nomor identifikasi internal</t>
         </is>
       </c>
     </row>
     <row r="15">
-      <c r="A15" t="inlineStr"/>
-      <c r="B15" t="inlineStr">
-        <is>
-          <t>- Tahun Pembuatan: Format 4 digit (contoh: 2020)</t>
+      <c r="A15" s="6" t="inlineStr"/>
+      <c r="B15" s="6" t="inlineStr">
+        <is>
+          <t>- Tahun Pembuatan: 4 digit (contoh: 2020)</t>
         </is>
       </c>
     </row>
     <row r="16">
-      <c r="A16" t="inlineStr"/>
-      <c r="B16" t="inlineStr">
-        <is>
-          <t>- Tanggal Expired STNK/KIR: Format YYYY-MM-DD</t>
+      <c r="A16" s="6" t="inlineStr"/>
+      <c r="B16" s="6" t="inlineStr">
+        <is>
+          <t>- Tanggal Expired STNK/KIR: Format YYYY-MM-DD (contoh: 2025-12-31)</t>
         </is>
       </c>
     </row>
     <row r="17">
-      <c r="A17" t="inlineStr"/>
-      <c r="B17" t="inlineStr"/>
+      <c r="A17" s="6" t="inlineStr"/>
+      <c r="B17" s="6" t="inlineStr"/>
     </row>
     <row r="18">
-      <c r="A18" t="inlineStr">
-        <is>
-          <t>4. Catatan:</t>
-        </is>
-      </c>
-      <c r="B18" t="inlineStr"/>
+      <c r="A18" s="6" t="inlineStr">
+        <is>
+          <t>4. Data Referensi:</t>
+        </is>
+      </c>
+      <c r="B18" s="6" t="inlineStr"/>
     </row>
     <row r="19">
-      <c r="A19" t="inlineStr"/>
-      <c r="B19" t="inlineStr">
-        <is>
-          <t>- Nomor polisi yang duplikat akan dilewati</t>
+      <c r="A19" s="6" t="inlineStr"/>
+      <c r="B19" s="6" t="inlineStr">
+        <is>
+          <t>- Lihat sheet 'Data Referensi' untuk daftar lengkap pilihan</t>
         </is>
       </c>
     </row>
     <row r="20">
-      <c r="A20" t="inlineStr"/>
-      <c r="B20" t="inlineStr">
-        <is>
-          <t>- Baris dengan data invalid akan dilaporkan sebagai error</t>
+      <c r="A20" s="6" t="inlineStr"/>
+      <c r="B20" s="6" t="inlineStr">
+        <is>
+          <t>- Dropdown otomatis terhubung ke data referensi</t>
         </is>
       </c>
     </row>
     <row r="21">
-      <c r="A21" t="inlineStr"/>
-      <c r="B21" t="inlineStr">
-        <is>
-          <t>- Tanggal expired akan digunakan untuk reminder otomatis</t>
+      <c r="A21" s="6" t="inlineStr"/>
+      <c r="B21" s="6" t="inlineStr">
+        <is>
+          <t>- Jika perlu menambah tipe kendaraan, tambahkan di sheet 'Data Referensi'</t>
         </is>
       </c>
     </row>
     <row r="22">
-      <c r="A22" t="inlineStr"/>
-      <c r="B22" t="inlineStr"/>
+      <c r="A22" s="6" t="inlineStr"/>
+      <c r="B22" s="6" t="inlineStr"/>
     </row>
     <row r="23">
-      <c r="A23" t="inlineStr">
-        <is>
-          <t>5. Contoh Data:</t>
-        </is>
-      </c>
-      <c r="B23" t="inlineStr"/>
+      <c r="A23" s="6" t="inlineStr">
+        <is>
+          <t>5. Catatan:</t>
+        </is>
+      </c>
+      <c r="B23" s="6" t="inlineStr"/>
     </row>
     <row r="24">
-      <c r="A24" t="inlineStr"/>
-      <c r="B24" t="inlineStr">
-        <is>
-          <t>Lihat sheet 'Data Kendaraan' untuk contoh format yang benar</t>
+      <c r="A24" s="6" t="inlineStr"/>
+      <c r="B24" s="6" t="inlineStr">
+        <is>
+          <t>- Nomor polisi duplikat akan dilewati</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="6" t="inlineStr"/>
+      <c r="B25" s="6" t="inlineStr">
+        <is>
+          <t>- Data invalid akan dilaporkan sebagai error</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="6" t="inlineStr"/>
+      <c r="B26" s="6" t="inlineStr">
+        <is>
+          <t>- Tanggal expired untuk reminder otomatis</t>
         </is>
       </c>
     </row>

</xml_diff>